<commit_message>
Alterado Mapa Lógico de Dados
</commit_message>
<xml_diff>
--- a/Mapa Lógico de Dados.xlsx
+++ b/Mapa Lógico de Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Desktop\AD(Local)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{21757207-576A-4E09-871A-D9ED9007BFD2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{53B59AB0-9726-402C-B855-4A3849A3D24C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{02890633-0B75-4B2B-BAAD-2E4BC6DBF0FF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="125">
   <si>
     <t>Table Name</t>
   </si>
@@ -283,6 +283,123 @@
   </si>
   <si>
     <t>Select s.country_region from suppliers where s.id = id_dim_employee</t>
+  </si>
+  <si>
+    <t>id_orders_facts</t>
+  </si>
+  <si>
+    <t>Fact</t>
+  </si>
+  <si>
+    <t>dw-northwind</t>
+  </si>
+  <si>
+    <t>unit_price</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>order_date</t>
+  </si>
+  <si>
+    <t>paid_date</t>
+  </si>
+  <si>
+    <t>shipped_date</t>
+  </si>
+  <si>
+    <t>DECIMAL(18,4)</t>
+  </si>
+  <si>
+    <t>order_details</t>
+  </si>
+  <si>
+    <t>Select p.unit_price from order_details where p.product_id = id_dim_products</t>
+  </si>
+  <si>
+    <t>Select p.quantity from order_details where p.product_id = id_dim_products</t>
+  </si>
+  <si>
+    <t>dim_time</t>
+  </si>
+  <si>
+    <t>where order_date = id_dim_time</t>
+  </si>
+  <si>
+    <t>id_dim_time</t>
+  </si>
+  <si>
+    <t>where paid_date = id_dim_time</t>
+  </si>
+  <si>
+    <t>where shipped_date = id_dim_time</t>
+  </si>
+  <si>
+    <t>where id_dim_products = dim_products.id_dim_products</t>
+  </si>
+  <si>
+    <t>where id_dim_customer = dim_customer.id_dim_customer</t>
+  </si>
+  <si>
+    <t>where id_dim_employee = dim_employee.id_dim_employee</t>
+  </si>
+  <si>
+    <t>purchase_order_fact</t>
+  </si>
+  <si>
+    <t>orders_fact</t>
+  </si>
+  <si>
+    <t>id_purchase_order_fact</t>
+  </si>
+  <si>
+    <t>unit_cost</t>
+  </si>
+  <si>
+    <t>submitted_date</t>
+  </si>
+  <si>
+    <t>payment_date</t>
+  </si>
+  <si>
+    <t>approved_date</t>
+  </si>
+  <si>
+    <t>purchase_order_details</t>
+  </si>
+  <si>
+    <t>select p.unit_cost from purchase_order_details where p.purchase_order_id = id_purchase_order_fact</t>
+  </si>
+  <si>
+    <t>select p.quantity from purchase_order_details where p.purchase_order_id = id_purchase_order_fact</t>
+  </si>
+  <si>
+    <t>Natural key from purchase_orders</t>
+  </si>
+  <si>
+    <t>purchase_orders</t>
+  </si>
+  <si>
+    <t>Natural key from orders</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>where submitted_date = id_dim_time</t>
+  </si>
+  <si>
+    <t>where payment_date = id_dim_time</t>
+  </si>
+  <si>
+    <t>where approved_date = id_dim_time</t>
+  </si>
+  <si>
+    <t>where id_dim_shipper = dim_shipper.id_dim_shipper</t>
+  </si>
+  <si>
+    <t>where id_dim_supplier = dim_supplier.id_dim_supplier</t>
   </si>
 </sst>
 </file>
@@ -434,6 +551,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -451,15 +577,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DF6B15-481C-4716-84ED-F779902A6AF0}">
-  <dimension ref="B2:K55"/>
+  <dimension ref="B2:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,20 +913,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="8" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15" t="s">
         <v>8</v>
       </c>
     </row>
@@ -841,7 +958,7 @@
       <c r="J3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="13"/>
+      <c r="K3" s="16"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -874,29 +991,29 @@
       </c>
     </row>
     <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="14" t="s">
+      <c r="D5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="14" t="s">
+      <c r="G5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -904,59 +1021,59 @@
       </c>
     </row>
     <row r="6" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="14" t="s">
+      <c r="G6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="14" t="s">
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="14" t="s">
+      <c r="G7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K7" s="5" t="s">
@@ -964,29 +1081,29 @@
       </c>
     </row>
     <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="D8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="14" t="s">
+      <c r="G8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K8" s="6" t="s">
@@ -1024,10 +1141,10 @@
       </c>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1043,7 +1160,7 @@
       <c r="H10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="8" t="s">
         <v>35</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -1087,26 +1204,26 @@
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="14" t="s">
+      <c r="G12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K12" s="7" t="s">
@@ -1114,59 +1231,59 @@
       </c>
     </row>
     <row r="13" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="14" t="s">
+      <c r="G13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="14" t="s">
+      <c r="D14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="14" t="s">
+      <c r="G14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K14" s="5" t="s">
@@ -1174,29 +1291,29 @@
       </c>
     </row>
     <row r="15" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="14" t="s">
+      <c r="D15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="14" t="s">
+      <c r="G15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K15" s="6" t="s">
@@ -1204,7 +1321,7 @@
       </c>
     </row>
     <row r="16" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1220,7 +1337,7 @@
       <c r="G16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="8" t="s">
         <v>39</v>
       </c>
       <c r="I16" s="4" t="s">
@@ -1234,10 +1351,10 @@
       </c>
     </row>
     <row r="17" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -1250,13 +1367,13 @@
       <c r="G17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K17" s="4" t="s">
@@ -1280,7 +1397,7 @@
       <c r="G18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="8" t="s">
         <v>48</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -1294,29 +1411,29 @@
       </c>
     </row>
     <row r="19" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="14" t="s">
+      <c r="D19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K19" s="4" t="s">
@@ -1324,29 +1441,29 @@
       </c>
     </row>
     <row r="20" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="8" t="s">
         <v>53</v>
       </c>
       <c r="K20" s="4" t="s">
@@ -1354,29 +1471,29 @@
       </c>
     </row>
     <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="8" t="s">
         <v>53</v>
       </c>
       <c r="K21" s="4" t="s">
@@ -1384,29 +1501,29 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="14" t="s">
+      <c r="D22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="J22" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K22" s="4" t="s">
@@ -1414,29 +1531,29 @@
       </c>
     </row>
     <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="J23" s="8" t="s">
         <v>59</v>
       </c>
       <c r="K23" s="4" t="s">
@@ -1444,29 +1561,29 @@
       </c>
     </row>
     <row r="24" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="14" t="s">
+      <c r="D24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K24" s="4" t="s">
@@ -1534,29 +1651,29 @@
       </c>
     </row>
     <row r="27" spans="2:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="I27" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="J27" s="14" t="s">
+      <c r="J27" s="8" t="s">
         <v>27</v>
       </c>
       <c r="K27" s="4" t="s">
@@ -1564,29 +1681,29 @@
       </c>
     </row>
     <row r="28" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="14" t="s">
+      <c r="D28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J28" s="14" t="s">
+      <c r="J28" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K28" s="4" t="s">
@@ -1594,29 +1711,29 @@
       </c>
     </row>
     <row r="29" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="14" t="s">
+      <c r="D29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="H29" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J29" s="14" t="s">
+      <c r="J29" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K29" s="4" t="s">
@@ -1624,29 +1741,29 @@
       </c>
     </row>
     <row r="30" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="14" t="s">
+      <c r="D30" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="I30" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="J30" s="14" t="s">
+      <c r="J30" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K30" s="4" t="s">
@@ -1654,29 +1771,29 @@
       </c>
     </row>
     <row r="31" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E31" s="14" t="s">
+      <c r="D31" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="I31" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K31" s="4" t="s">
@@ -1693,7 +1810,7 @@
       <c r="D32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="1"/>
@@ -1723,7 +1840,7 @@
       <c r="D33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="1"/>
@@ -1736,7 +1853,7 @@
       <c r="I33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K33" s="4" t="s">
@@ -1750,10 +1867,10 @@
       <c r="C34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F34" s="1"/>
@@ -1766,7 +1883,7 @@
       <c r="I34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J34" s="14" t="s">
+      <c r="J34" s="8" t="s">
         <v>27</v>
       </c>
       <c r="K34" s="4" t="s">
@@ -1780,10 +1897,10 @@
       <c r="C35" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="14" t="s">
+      <c r="D35" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="1"/>
@@ -1796,7 +1913,7 @@
       <c r="I35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J35" s="14" t="s">
+      <c r="J35" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K35" s="4" t="s">
@@ -1810,10 +1927,10 @@
       <c r="C36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="14" t="s">
+      <c r="D36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F36" s="1"/>
@@ -1826,7 +1943,7 @@
       <c r="I36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J36" s="14" t="s">
+      <c r="J36" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K36" s="4" t="s">
@@ -1840,10 +1957,10 @@
       <c r="C37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="14" t="s">
+      <c r="D37" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F37" s="1"/>
@@ -1856,7 +1973,7 @@
       <c r="I37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J37" s="14" t="s">
+      <c r="J37" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K37" s="4" t="s">
@@ -1870,10 +1987,10 @@
       <c r="C38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="14" t="s">
+      <c r="D38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F38" s="1"/>
@@ -1886,7 +2003,7 @@
       <c r="I38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J38" s="14" t="s">
+      <c r="J38" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K38" s="4" t="s">
@@ -1894,208 +2011,574 @@
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="G39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="G40" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
+      <c r="G41" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K41" s="10" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
+      <c r="G42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
+      <c r="G43" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
+      <c r="G44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K45" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K46" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J48" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K48" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
+      <c r="B49" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J50" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K50" s="10" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
+      <c r="B51" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
+      <c r="B52" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
+      <c r="B53" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K54" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B55" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K56" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B57" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>